<commit_message>
update note on TMDS cut out
</commit_message>
<xml_diff>
--- a/EC/Train Runs 2016-05-16 (FRA Format).xlsx
+++ b/EC/Train Runs 2016-05-16 (FRA Format).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" tabRatio="845" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" tabRatio="845" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Summary" sheetId="15" r:id="rId1"/>
@@ -4434,9 +4434,6 @@
     <t>Onboard entered a failsafe state that caused train comm outage</t>
   </si>
   <si>
-    <t>Train was cut out by message from dispatch system</t>
-  </si>
-  <si>
     <t>Wayside link failure</t>
   </si>
   <si>
@@ -5737,6 +5734,9 @@
   </si>
   <si>
     <t>Routing at DUS Signal 2N</t>
+  </si>
+  <si>
+    <t>Onboard entered a failsafe state that caused the dispatch system to cut it out</t>
   </si>
 </sst>
 </file>
@@ -6266,53 +6266,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="220">
+  <dxfs count="208">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6369,6 +6327,48 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7723,90 +7723,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8010,7 +7926,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8034,11 +7950,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016_2" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016_1" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Denver Train Runs 04122016_2" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11942,8 +11858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14292,7 +14208,7 @@
         <v>2.733796297252411E-2</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>1376</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14506,7 +14422,7 @@
         <v>2.9872685190639459E-2</v>
       </c>
       <c r="G113" s="10" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14676,7 +14592,7 @@
         <v>3.0752314814890269E-2</v>
       </c>
       <c r="G121" s="10" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14699,7 +14615,7 @@
         <v>2.4189814816054422E-2</v>
       </c>
       <c r="G122" s="10" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14745,7 +14661,7 @@
         <v>2.6087962964083999E-2</v>
       </c>
       <c r="G124" s="10" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -15047,7 +14963,7 @@
         <v>9.9999999947613105E-3</v>
       </c>
       <c r="G138" s="10" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="I138" s="2"/>
       <c r="J138" s="2"/>
@@ -15634,7 +15550,7 @@
     </row>
     <row r="4" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B4" s="6">
         <v>4032</v>
@@ -15668,7 +15584,7 @@
     </row>
     <row r="5" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B5" s="6">
         <v>4040</v>
@@ -15705,7 +15621,7 @@
     </row>
     <row r="6" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B6" s="6">
         <v>4023</v>
@@ -15742,7 +15658,7 @@
     </row>
     <row r="7" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B7" s="6">
         <v>4016</v>
@@ -15779,7 +15695,7 @@
     </row>
     <row r="8" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B8" s="6">
         <v>4026</v>
@@ -15816,7 +15732,7 @@
     </row>
     <row r="9" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B9" s="6">
         <v>4038</v>
@@ -15852,7 +15768,7 @@
     </row>
     <row r="10" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B10" s="6">
         <v>4037</v>
@@ -15873,7 +15789,7 @@
     </row>
     <row r="11" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B11" s="6">
         <v>4014</v>
@@ -15894,7 +15810,7 @@
     </row>
     <row r="12" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="B12" s="6">
         <v>4013</v>
@@ -15915,7 +15831,7 @@
     </row>
     <row r="13" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B13" s="6">
         <v>4011</v>
@@ -15936,7 +15852,7 @@
     </row>
     <row r="14" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B14" s="6">
         <v>4012</v>
@@ -15957,7 +15873,7 @@
     </row>
     <row r="15" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B15" s="6">
         <v>4031</v>
@@ -15978,7 +15894,7 @@
     </row>
     <row r="16" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="B16" s="6">
         <v>4032</v>
@@ -15999,7 +15915,7 @@
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="B17" s="6">
         <v>4040</v>
@@ -16020,7 +15936,7 @@
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B18" s="6">
         <v>4039</v>
@@ -16041,7 +15957,7 @@
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="B19" s="6">
         <v>4024</v>
@@ -16062,7 +15978,7 @@
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="B20" s="6">
         <v>4023</v>
@@ -16083,7 +15999,7 @@
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="B21" s="6">
         <v>4016</v>
@@ -16104,7 +16020,7 @@
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B22" s="6">
         <v>4015</v>
@@ -16125,7 +16041,7 @@
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="B23" s="6">
         <v>4038</v>
@@ -16146,7 +16062,7 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="B24" s="6">
         <v>4037</v>
@@ -16167,7 +16083,7 @@
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B25" s="6">
         <v>4014</v>
@@ -16188,7 +16104,7 @@
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B26" s="6">
         <v>4013</v>
@@ -16209,7 +16125,7 @@
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B27" s="6">
         <v>4011</v>
@@ -16232,7 +16148,7 @@
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B28" s="6">
         <v>4012</v>
@@ -16253,7 +16169,7 @@
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B29" s="6">
         <v>4031</v>
@@ -16274,7 +16190,7 @@
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B30" s="6">
         <v>4032</v>
@@ -16295,7 +16211,7 @@
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B31" s="6">
         <v>4040</v>
@@ -16316,7 +16232,7 @@
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B32" s="6">
         <v>4039</v>
@@ -16337,7 +16253,7 @@
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B33" s="6">
         <v>4024</v>
@@ -16358,7 +16274,7 @@
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B34" s="6">
         <v>4023</v>
@@ -16379,7 +16295,7 @@
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B35" s="6">
         <v>4016</v>
@@ -16400,7 +16316,7 @@
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B36" s="6">
         <v>4015</v>
@@ -16421,7 +16337,7 @@
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B37" s="6">
         <v>4038</v>
@@ -16442,7 +16358,7 @@
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="B38" s="6">
         <v>4037</v>
@@ -16463,7 +16379,7 @@
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B39" s="6">
         <v>4014</v>
@@ -16484,7 +16400,7 @@
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B40" s="6">
         <v>4013</v>
@@ -16505,7 +16421,7 @@
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B41" s="6">
         <v>4011</v>
@@ -16526,7 +16442,7 @@
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B42" s="6">
         <v>4012</v>
@@ -16547,7 +16463,7 @@
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B43" s="6">
         <v>4031</v>
@@ -16568,7 +16484,7 @@
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B44" s="6">
         <v>4032</v>
@@ -16589,7 +16505,7 @@
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B45" s="6">
         <v>4040</v>
@@ -16610,7 +16526,7 @@
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B46" s="6">
         <v>4039</v>
@@ -16631,7 +16547,7 @@
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B47" s="6">
         <v>4024</v>
@@ -16652,7 +16568,7 @@
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B48" s="6">
         <v>4023</v>
@@ -16673,7 +16589,7 @@
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B49" s="6">
         <v>4016</v>
@@ -16696,7 +16612,7 @@
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B50" s="6">
         <v>4015</v>
@@ -16717,7 +16633,7 @@
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B51" s="6">
         <v>4038</v>
@@ -16738,7 +16654,7 @@
     </row>
     <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B52" s="6">
         <v>4037</v>
@@ -16759,7 +16675,7 @@
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B53" s="6">
         <v>4014</v>
@@ -16780,7 +16696,7 @@
     </row>
     <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B54" s="6">
         <v>4013</v>
@@ -16801,7 +16717,7 @@
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B55" s="6">
         <v>4011</v>
@@ -16822,7 +16738,7 @@
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B56" s="6">
         <v>4012</v>
@@ -16843,7 +16759,7 @@
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="B57" s="6">
         <v>4031</v>
@@ -16864,7 +16780,7 @@
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B58" s="6">
         <v>4032</v>
@@ -16885,7 +16801,7 @@
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="B59" s="6">
         <v>4040</v>
@@ -16906,7 +16822,7 @@
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B60" s="6">
         <v>4039</v>
@@ -16927,7 +16843,7 @@
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B61" s="6">
         <v>4024</v>
@@ -16948,7 +16864,7 @@
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B62" s="6">
         <v>4023</v>
@@ -16969,7 +16885,7 @@
     </row>
     <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="B63" s="6">
         <v>4015</v>
@@ -16990,7 +16906,7 @@
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B64" s="6">
         <v>4038</v>
@@ -17011,7 +16927,7 @@
     </row>
     <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B65" s="6">
         <v>4037</v>
@@ -17032,7 +16948,7 @@
     </row>
     <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B66" s="6">
         <v>4014</v>
@@ -17053,7 +16969,7 @@
     </row>
     <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B67" s="6">
         <v>4013</v>
@@ -17074,7 +16990,7 @@
     </row>
     <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B68" s="6">
         <v>4011</v>
@@ -17095,7 +17011,7 @@
     </row>
     <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B69" s="6">
         <v>4012</v>
@@ -17116,7 +17032,7 @@
     </row>
     <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B70" s="6">
         <v>4031</v>
@@ -17137,7 +17053,7 @@
     </row>
     <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B71" s="6">
         <v>4032</v>
@@ -17158,7 +17074,7 @@
     </row>
     <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B72" s="6">
         <v>4040</v>
@@ -17179,7 +17095,7 @@
     </row>
     <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B73" s="6">
         <v>4039</v>
@@ -17200,7 +17116,7 @@
     </row>
     <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B74" s="6">
         <v>4025</v>
@@ -17221,7 +17137,7 @@
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B75" s="6">
         <v>4026</v>
@@ -17242,7 +17158,7 @@
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B76" s="6">
         <v>4016</v>
@@ -17263,7 +17179,7 @@
     </row>
     <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B77" s="6">
         <v>4015</v>
@@ -17284,7 +17200,7 @@
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B78" s="6">
         <v>4038</v>
@@ -17305,7 +17221,7 @@
     </row>
     <row r="79" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B79" s="6">
         <v>4037</v>
@@ -17326,7 +17242,7 @@
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B80" s="6">
         <v>4014</v>
@@ -17347,7 +17263,7 @@
     </row>
     <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B81" s="6">
         <v>4013</v>
@@ -17368,7 +17284,7 @@
     </row>
     <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B82" s="6">
         <v>4011</v>
@@ -17389,7 +17305,7 @@
     </row>
     <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B83" s="6">
         <v>4012</v>
@@ -17410,7 +17326,7 @@
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B84" s="6">
         <v>4031</v>
@@ -17431,7 +17347,7 @@
     </row>
     <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B85" s="6">
         <v>4032</v>
@@ -17452,7 +17368,7 @@
     </row>
     <row r="86" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B86" s="6">
         <v>4040</v>
@@ -17473,7 +17389,7 @@
     </row>
     <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B87" s="6">
         <v>4039</v>
@@ -17494,7 +17410,7 @@
     </row>
     <row r="88" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B88" s="6">
         <v>4025</v>
@@ -17515,7 +17431,7 @@
     </row>
     <row r="89" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B89" s="6">
         <v>4026</v>
@@ -17536,7 +17452,7 @@
     </row>
     <row r="90" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B90" s="6">
         <v>4016</v>
@@ -17557,7 +17473,7 @@
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B91" s="6">
         <v>4015</v>
@@ -17578,7 +17494,7 @@
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B92" s="6">
         <v>4038</v>
@@ -17599,7 +17515,7 @@
     </row>
     <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B93" s="6">
         <v>4037</v>
@@ -17620,7 +17536,7 @@
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B94" s="6">
         <v>4014</v>
@@ -17641,7 +17557,7 @@
     </row>
     <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B95" s="6">
         <v>4013</v>
@@ -17662,7 +17578,7 @@
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B96" s="6">
         <v>4011</v>
@@ -17683,7 +17599,7 @@
     </row>
     <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B97" s="6">
         <v>4012</v>
@@ -17704,7 +17620,7 @@
     </row>
     <row r="98" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B98" s="6">
         <v>4031</v>
@@ -17725,7 +17641,7 @@
     </row>
     <row r="99" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B99" s="6">
         <v>4032</v>
@@ -17746,7 +17662,7 @@
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B100" s="6">
         <v>4040</v>
@@ -17767,7 +17683,7 @@
     </row>
     <row r="101" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B101" s="6">
         <v>4039</v>
@@ -17788,7 +17704,7 @@
     </row>
     <row r="102" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B102" s="6">
         <v>4025</v>
@@ -17809,7 +17725,7 @@
     </row>
     <row r="103" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B103" s="6">
         <v>4026</v>
@@ -17830,7 +17746,7 @@
     </row>
     <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B104" s="6">
         <v>4016</v>
@@ -17851,7 +17767,7 @@
     </row>
     <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B105" s="6">
         <v>4015</v>
@@ -17872,7 +17788,7 @@
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B106" s="6">
         <v>4038</v>
@@ -17893,7 +17809,7 @@
     </row>
     <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B107" s="6">
         <v>4037</v>
@@ -17914,7 +17830,7 @@
     </row>
     <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B108" s="6">
         <v>4014</v>
@@ -17935,7 +17851,7 @@
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B109" s="6">
         <v>4013</v>
@@ -17956,7 +17872,7 @@
     </row>
     <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B110" s="6">
         <v>4011</v>
@@ -17977,7 +17893,7 @@
     </row>
     <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="B111" s="6">
         <v>4012</v>
@@ -17998,7 +17914,7 @@
     </row>
     <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="B112" s="6">
         <v>4031</v>
@@ -18019,7 +17935,7 @@
     </row>
     <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B113" s="6">
         <v>4032</v>
@@ -18040,7 +17956,7 @@
     </row>
     <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B114" s="6">
         <v>4040</v>
@@ -18061,7 +17977,7 @@
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B115" s="6">
         <v>4039</v>
@@ -18082,7 +17998,7 @@
     </row>
     <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B116" s="6">
         <v>4025</v>
@@ -18103,7 +18019,7 @@
     </row>
     <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="B117" s="6">
         <v>4026</v>
@@ -18124,7 +18040,7 @@
     </row>
     <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="B118" s="6">
         <v>4016</v>
@@ -18145,7 +18061,7 @@
     </row>
     <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B119" s="6">
         <v>4015</v>
@@ -18166,7 +18082,7 @@
     </row>
     <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B120" s="6">
         <v>4038</v>
@@ -18187,7 +18103,7 @@
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="B121" s="6">
         <v>4037</v>
@@ -18208,7 +18124,7 @@
     </row>
     <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B122" s="6">
         <v>4011</v>
@@ -18229,7 +18145,7 @@
     </row>
     <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B123" s="6">
         <v>4012</v>
@@ -18250,7 +18166,7 @@
     </row>
     <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="B124" s="6">
         <v>4040</v>
@@ -18271,7 +18187,7 @@
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B125" s="6">
         <v>4039</v>
@@ -18292,7 +18208,7 @@
     </row>
     <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B126" s="6">
         <v>4016</v>
@@ -18313,7 +18229,7 @@
     </row>
     <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B127" s="6">
         <v>4015</v>
@@ -18334,7 +18250,7 @@
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B128" s="6">
         <v>4038</v>
@@ -18355,7 +18271,7 @@
     </row>
     <row r="129" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B129" s="6">
         <v>4037</v>
@@ -18376,7 +18292,7 @@
     </row>
     <row r="130" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B130" s="6">
         <v>4024</v>
@@ -18397,7 +18313,7 @@
     </row>
     <row r="131" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B131" s="6">
         <v>4023</v>
@@ -18418,7 +18334,7 @@
     </row>
     <row r="132" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B132" s="6">
         <v>4040</v>
@@ -18439,7 +18355,7 @@
     </row>
     <row r="133" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B133" s="6">
         <v>4039</v>
@@ -18460,7 +18376,7 @@
     </row>
     <row r="134" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B134" s="6">
         <v>4016</v>
@@ -18481,7 +18397,7 @@
     </row>
     <row r="135" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B135" s="6">
         <v>4015</v>
@@ -18502,7 +18418,7 @@
     </row>
     <row r="136" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B136" s="6">
         <v>4038</v>
@@ -18523,7 +18439,7 @@
     </row>
     <row r="137" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B137" s="6">
         <v>4037</v>
@@ -18544,7 +18460,7 @@
     </row>
     <row r="138" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B138" s="6">
         <v>4024</v>
@@ -18566,7 +18482,7 @@
     </row>
     <row r="139" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B139" s="6">
         <v>4023</v>
@@ -18588,7 +18504,7 @@
     </row>
     <row r="140" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="B140" s="6">
         <v>4040</v>
@@ -18610,7 +18526,7 @@
     </row>
     <row r="141" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B141" s="6">
         <v>4039</v>
@@ -18632,7 +18548,7 @@
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B142" s="6">
         <v>4016</v>
@@ -18655,7 +18571,7 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B143" s="6">
         <v>4015</v>
@@ -18679,7 +18595,7 @@
     </row>
     <row r="144" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B144" s="6">
         <v>4038</v>
@@ -18705,7 +18621,7 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B145" s="6">
         <v>4037</v>
@@ -18728,7 +18644,7 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="B146" s="6">
         <v>4024</v>
@@ -18751,7 +18667,7 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B147" s="6">
         <v>4023</v>
@@ -19177,7 +19093,7 @@
     </row>
     <row r="4" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B4" s="6">
         <v>4032</v>
@@ -19211,7 +19127,7 @@
     </row>
     <row r="5" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B5" s="6">
         <v>4007</v>
@@ -19248,7 +19164,7 @@
     </row>
     <row r="6" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B6" s="6">
         <v>4017</v>
@@ -19266,7 +19182,7 @@
         <v>2.156249999825377E-2</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>15</v>
@@ -19287,7 +19203,7 @@
     </row>
     <row r="7" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B7" s="6">
         <v>4025</v>
@@ -19305,7 +19221,7 @@
         <v>2.3587962961755693E-2</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>9</v>
@@ -19326,7 +19242,7 @@
     </row>
     <row r="8" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B8" s="6">
         <v>4030</v>
@@ -19363,7 +19279,7 @@
     </row>
     <row r="9" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B9" s="6">
         <v>4016</v>
@@ -19399,7 +19315,7 @@
     </row>
     <row r="10" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B10" s="6">
         <v>4015</v>
@@ -19420,7 +19336,7 @@
     </row>
     <row r="11" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B11" s="6">
         <v>4040</v>
@@ -19441,7 +19357,7 @@
     </row>
     <row r="12" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B12" s="6">
         <v>4039</v>
@@ -19462,7 +19378,7 @@
     </row>
     <row r="13" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B13" s="6">
         <v>4014</v>
@@ -19483,7 +19399,7 @@
     </row>
     <row r="14" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B14" s="6">
         <v>4013</v>
@@ -19504,7 +19420,7 @@
     </row>
     <row r="15" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B15" s="6">
         <v>4031</v>
@@ -19525,7 +19441,7 @@
     </row>
     <row r="16" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B16" s="6">
         <v>4032</v>
@@ -19546,7 +19462,7 @@
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="B17" s="6">
         <v>4007</v>
@@ -19567,7 +19483,7 @@
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B18" s="6">
         <v>4008</v>
@@ -19588,7 +19504,7 @@
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="B19" s="6">
         <v>4018</v>
@@ -19609,7 +19525,7 @@
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B20" s="6">
         <v>4017</v>
@@ -19630,7 +19546,7 @@
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="B21" s="6">
         <v>4029</v>
@@ -19651,7 +19567,7 @@
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B22" s="6">
         <v>4030</v>
@@ -19674,7 +19590,7 @@
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B23" s="6">
         <v>4016</v>
@@ -19695,7 +19611,7 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B24" s="6">
         <v>4015</v>
@@ -19716,7 +19632,7 @@
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B25" s="6">
         <v>4040</v>
@@ -19737,7 +19653,7 @@
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="B26" s="6">
         <v>4039</v>
@@ -19755,12 +19671,12 @@
         <v>1.6365740746550728E-2</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="B27" s="6">
         <v>4014</v>
@@ -19781,7 +19697,7 @@
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B28" s="6">
         <v>4013</v>
@@ -19802,7 +19718,7 @@
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B29" s="6">
         <v>4031</v>
@@ -19823,7 +19739,7 @@
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B30" s="6">
         <v>4032</v>
@@ -19844,7 +19760,7 @@
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="B31" s="6">
         <v>4007</v>
@@ -19865,7 +19781,7 @@
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B32" s="6">
         <v>4008</v>
@@ -19886,7 +19802,7 @@
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B33" s="6">
         <v>4018</v>
@@ -19907,7 +19823,7 @@
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B34" s="6">
         <v>4017</v>
@@ -19928,7 +19844,7 @@
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B35" s="6">
         <v>4024</v>
@@ -19949,7 +19865,7 @@
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B36" s="6">
         <v>4023</v>
@@ -19970,7 +19886,7 @@
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="B37" s="6">
         <v>4016</v>
@@ -19991,7 +19907,7 @@
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="B38" s="6">
         <v>4015</v>
@@ -20012,7 +19928,7 @@
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="B39" s="6">
         <v>4040</v>
@@ -20033,7 +19949,7 @@
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="B40" s="6">
         <v>4039</v>
@@ -20054,7 +19970,7 @@
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B41" s="6">
         <v>4014</v>
@@ -20075,7 +19991,7 @@
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="B42" s="6">
         <v>4013</v>
@@ -20096,7 +20012,7 @@
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="B43" s="6">
         <v>4031</v>
@@ -20117,7 +20033,7 @@
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="B44" s="6">
         <v>4032</v>
@@ -20138,7 +20054,7 @@
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="B45" s="6">
         <v>4007</v>
@@ -20159,7 +20075,7 @@
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="B46" s="6">
         <v>4008</v>
@@ -20180,7 +20096,7 @@
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="B47" s="6">
         <v>4018</v>
@@ -20201,7 +20117,7 @@
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="B48" s="6">
         <v>4017</v>
@@ -20222,7 +20138,7 @@
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="B49" s="6">
         <v>4024</v>
@@ -20243,7 +20159,7 @@
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="B50" s="6">
         <v>4023</v>
@@ -20264,7 +20180,7 @@
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B51" s="6">
         <v>4016</v>
@@ -20285,7 +20201,7 @@
     </row>
     <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B52" s="6">
         <v>4015</v>
@@ -20306,7 +20222,7 @@
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="B53" s="6">
         <v>4040</v>
@@ -20327,7 +20243,7 @@
     </row>
     <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="B54" s="6">
         <v>4039</v>
@@ -20348,7 +20264,7 @@
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="B55" s="6">
         <v>4014</v>
@@ -20369,7 +20285,7 @@
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="B56" s="6">
         <v>4013</v>
@@ -20390,7 +20306,7 @@
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="B57" s="6">
         <v>4031</v>
@@ -20411,7 +20327,7 @@
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="B58" s="6">
         <v>4032</v>
@@ -20432,7 +20348,7 @@
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B59" s="6">
         <v>4007</v>
@@ -20453,7 +20369,7 @@
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B60" s="6">
         <v>4008</v>
@@ -20474,7 +20390,7 @@
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B61" s="6">
         <v>4018</v>
@@ -20495,7 +20411,7 @@
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="B62" s="6">
         <v>4017</v>
@@ -20516,7 +20432,7 @@
     </row>
     <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B63" s="6">
         <v>4024</v>
@@ -20537,7 +20453,7 @@
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B64" s="6">
         <v>4023</v>
@@ -20558,7 +20474,7 @@
     </row>
     <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B65" s="6">
         <v>4016</v>
@@ -20579,7 +20495,7 @@
     </row>
     <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B66" s="6">
         <v>4015</v>
@@ -20600,7 +20516,7 @@
     </row>
     <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B67" s="6">
         <v>4040</v>
@@ -20621,7 +20537,7 @@
     </row>
     <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="B68" s="6">
         <v>4039</v>
@@ -20642,7 +20558,7 @@
     </row>
     <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B69" s="6">
         <v>4014</v>
@@ -20663,7 +20579,7 @@
     </row>
     <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="B70" s="6">
         <v>4013</v>
@@ -20684,7 +20600,7 @@
     </row>
     <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="B71" s="6">
         <v>4031</v>
@@ -20705,7 +20621,7 @@
     </row>
     <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B72" s="6">
         <v>4032</v>
@@ -20726,7 +20642,7 @@
     </row>
     <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B73" s="6">
         <v>4007</v>
@@ -20747,7 +20663,7 @@
     </row>
     <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B74" s="6">
         <v>4008</v>
@@ -20768,7 +20684,7 @@
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B75" s="6">
         <v>4018</v>
@@ -20789,7 +20705,7 @@
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B76" s="6">
         <v>4017</v>
@@ -20810,7 +20726,7 @@
     </row>
     <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B77" s="6">
         <v>4024</v>
@@ -20831,7 +20747,7 @@
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B78" s="6">
         <v>4023</v>
@@ -20852,7 +20768,7 @@
     </row>
     <row r="79" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B79" s="6">
         <v>4016</v>
@@ -20873,7 +20789,7 @@
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B80" s="6">
         <v>4015</v>
@@ -20894,7 +20810,7 @@
     </row>
     <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B81" s="6">
         <v>4040</v>
@@ -20915,7 +20831,7 @@
     </row>
     <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="B82" s="6">
         <v>4039</v>
@@ -20936,7 +20852,7 @@
     </row>
     <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="B83" s="6">
         <v>4014</v>
@@ -20957,7 +20873,7 @@
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="B84" s="6">
         <v>4013</v>
@@ -20978,7 +20894,7 @@
     </row>
     <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B85" s="6">
         <v>4031</v>
@@ -20999,7 +20915,7 @@
     </row>
     <row r="86" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B86" s="6">
         <v>4032</v>
@@ -21020,7 +20936,7 @@
     </row>
     <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="B87" s="6">
         <v>4007</v>
@@ -21041,7 +20957,7 @@
     </row>
     <row r="88" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B88" s="6">
         <v>4008</v>
@@ -21062,7 +20978,7 @@
     </row>
     <row r="89" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="B89" s="6">
         <v>4018</v>
@@ -21083,7 +20999,7 @@
     </row>
     <row r="90" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="B90" s="6">
         <v>4017</v>
@@ -21104,7 +21020,7 @@
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="B91" s="6">
         <v>4024</v>
@@ -21125,7 +21041,7 @@
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="B92" s="6">
         <v>4023</v>
@@ -21146,7 +21062,7 @@
     </row>
     <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="B93" s="6">
         <v>4016</v>
@@ -21167,7 +21083,7 @@
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B94" s="6">
         <v>4015</v>
@@ -21188,7 +21104,7 @@
     </row>
     <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B95" s="6">
         <v>4040</v>
@@ -21209,7 +21125,7 @@
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B96" s="6">
         <v>4039</v>
@@ -21230,7 +21146,7 @@
     </row>
     <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B97" s="6">
         <v>4014</v>
@@ -21251,7 +21167,7 @@
     </row>
     <row r="98" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B98" s="6">
         <v>4013</v>
@@ -21272,7 +21188,7 @@
     </row>
     <row r="99" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B99" s="6">
         <v>4031</v>
@@ -21293,7 +21209,7 @@
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="B100" s="6">
         <v>4032</v>
@@ -21314,7 +21230,7 @@
     </row>
     <row r="101" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="B101" s="6">
         <v>4007</v>
@@ -21337,7 +21253,7 @@
     </row>
     <row r="102" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="B102" s="6">
         <v>4008</v>
@@ -21358,7 +21274,7 @@
     </row>
     <row r="103" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="B103" s="6">
         <v>4018</v>
@@ -21379,7 +21295,7 @@
     </row>
     <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B104" s="6">
         <v>4017</v>
@@ -21400,7 +21316,7 @@
     </row>
     <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="B105" s="6">
         <v>4024</v>
@@ -21421,7 +21337,7 @@
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B106" s="6">
         <v>4023</v>
@@ -21442,7 +21358,7 @@
     </row>
     <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B107" s="6">
         <v>4016</v>
@@ -21463,7 +21379,7 @@
     </row>
     <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B108" s="6">
         <v>4015</v>
@@ -21484,7 +21400,7 @@
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B109" s="6">
         <v>4040</v>
@@ -21505,7 +21421,7 @@
     </row>
     <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B110" s="6">
         <v>4039</v>
@@ -21523,12 +21439,12 @@
         <v>1.7835648148320615E-2</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B111" s="6">
         <v>4014</v>
@@ -21549,7 +21465,7 @@
     </row>
     <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B112" s="6">
         <v>4013</v>
@@ -21570,7 +21486,7 @@
     </row>
     <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="B113" s="6">
         <v>4031</v>
@@ -21591,7 +21507,7 @@
     </row>
     <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B114" s="6">
         <v>4032</v>
@@ -21612,7 +21528,7 @@
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="B115" s="6">
         <v>4029</v>
@@ -21633,7 +21549,7 @@
     </row>
     <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B116" s="6">
         <v>4030</v>
@@ -21654,7 +21570,7 @@
     </row>
     <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B117" s="6">
         <v>4018</v>
@@ -21675,7 +21591,7 @@
     </row>
     <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="B118" s="6">
         <v>4017</v>
@@ -21696,7 +21612,7 @@
     </row>
     <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B119" s="6">
         <v>4024</v>
@@ -21717,7 +21633,7 @@
     </row>
     <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B120" s="6">
         <v>4023</v>
@@ -21738,7 +21654,7 @@
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="B121" s="6">
         <v>4016</v>
@@ -21759,7 +21675,7 @@
     </row>
     <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B122" s="6">
         <v>4015</v>
@@ -21780,7 +21696,7 @@
     </row>
     <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="B123" s="6">
         <v>4014</v>
@@ -21801,7 +21717,7 @@
     </row>
     <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="B124" s="6">
         <v>4013</v>
@@ -21822,7 +21738,7 @@
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="B125" s="6">
         <v>4029</v>
@@ -21843,7 +21759,7 @@
     </row>
     <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B126" s="6">
         <v>4030</v>
@@ -21864,7 +21780,7 @@
     </row>
     <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="B127" s="6">
         <v>4024</v>
@@ -21885,7 +21801,7 @@
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="B128" s="6">
         <v>4023</v>
@@ -21903,12 +21819,12 @@
         <v>1.1585648149775807E-2</v>
       </c>
       <c r="G128" s="10" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="129" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="B129" s="6">
         <v>4016</v>
@@ -21929,7 +21845,7 @@
     </row>
     <row r="130" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B130" s="6">
         <v>4015</v>
@@ -21947,12 +21863,12 @@
         <v>1.1481481480586808E-2</v>
       </c>
       <c r="G130" s="10" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="131" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B131" s="6">
         <v>4014</v>
@@ -21970,12 +21886,12 @@
         <v>8.2523148157633841E-3</v>
       </c>
       <c r="G131" s="10" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="132" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B132" s="6">
         <v>4029</v>
@@ -21993,12 +21909,12 @@
         <v>2.2418981476221234E-2</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="133" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B133" s="6">
         <v>4007</v>
@@ -22016,12 +21932,12 @@
         <v>5.7870370073942468E-4</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="134" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B134" s="6">
         <v>4030</v>
@@ -22042,7 +21958,7 @@
     </row>
     <row r="135" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B135" s="6">
         <v>4024</v>
@@ -22063,7 +21979,7 @@
     </row>
     <row r="136" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B136" s="6">
         <v>4008</v>
@@ -22084,7 +22000,7 @@
     </row>
     <row r="137" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B137" s="6">
         <v>4016</v>
@@ -22105,7 +22021,7 @@
     </row>
     <row r="138" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B138" s="6">
         <v>4023</v>
@@ -22127,7 +22043,7 @@
     </row>
     <row r="139" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B139" s="6">
         <v>4014</v>
@@ -22149,7 +22065,7 @@
     </row>
     <row r="140" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B140" s="6">
         <v>4015</v>
@@ -22171,7 +22087,7 @@
     </row>
     <row r="141" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B141" s="6">
         <v>4029</v>
@@ -22193,7 +22109,7 @@
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B142" s="6">
         <v>4013</v>
@@ -22216,7 +22132,7 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B143" s="6">
         <v>4007</v>
@@ -22240,7 +22156,7 @@
     </row>
     <row r="144" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B144" s="6">
         <v>4030</v>
@@ -22614,8 +22530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22729,7 +22645,7 @@
     </row>
     <row r="3" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="B3" s="6">
         <v>4011</v>
@@ -22761,7 +22677,7 @@
     </row>
     <row r="4" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="B4" s="6">
         <v>4019</v>
@@ -22797,7 +22713,7 @@
     </row>
     <row r="5" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="B5" s="6">
         <v>4031</v>
@@ -22836,7 +22752,7 @@
     </row>
     <row r="6" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B6" s="6">
         <v>4010</v>
@@ -22875,7 +22791,7 @@
     </row>
     <row r="7" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="B7" s="6">
         <v>4040</v>
@@ -22914,7 +22830,7 @@
     </row>
     <row r="8" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="B8" s="6">
         <v>4043</v>
@@ -22953,7 +22869,7 @@
     </row>
     <row r="9" spans="1:65" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="B9" s="6">
         <v>4024</v>
@@ -22991,7 +22907,7 @@
     </row>
     <row r="10" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="B10" s="6">
         <v>4023</v>
@@ -23014,7 +22930,7 @@
     </row>
     <row r="11" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B11" s="6">
         <v>4016</v>
@@ -23037,7 +22953,7 @@
     </row>
     <row r="12" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="B12" s="6">
         <v>4015</v>
@@ -23060,7 +22976,7 @@
     </row>
     <row r="13" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="B13" s="6">
         <v>4011</v>
@@ -23083,7 +22999,7 @@
     </row>
     <row r="14" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="B14" s="6">
         <v>4012</v>
@@ -23106,7 +23022,7 @@
     </row>
     <row r="15" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B15" s="6">
         <v>4020</v>
@@ -23129,7 +23045,7 @@
     </row>
     <row r="16" spans="1:65" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="B16" s="6">
         <v>4019</v>
@@ -23152,7 +23068,7 @@
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="B17" s="6">
         <v>4031</v>
@@ -23175,7 +23091,7 @@
     </row>
     <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="B18" s="6">
         <v>4032</v>
@@ -23198,7 +23114,7 @@
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="B19" s="6">
         <v>4009</v>
@@ -23221,7 +23137,7 @@
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="B20" s="6">
         <v>4010</v>
@@ -23244,7 +23160,7 @@
     </row>
     <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="B21" s="6">
         <v>4040</v>
@@ -23267,7 +23183,7 @@
     </row>
     <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="B22" s="6">
         <v>4039</v>
@@ -23290,7 +23206,7 @@
     </row>
     <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="B23" s="6">
         <v>4024</v>
@@ -23313,7 +23229,7 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="B24" s="6">
         <v>4023</v>
@@ -23336,7 +23252,7 @@
     </row>
     <row r="25" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="B25" s="6">
         <v>4016</v>
@@ -23359,7 +23275,7 @@
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="B26" s="6">
         <v>4015</v>
@@ -23382,7 +23298,7 @@
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="B27" s="6">
         <v>4011</v>
@@ -23405,7 +23321,7 @@
     </row>
     <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B28" s="6">
         <v>4012</v>
@@ -23428,7 +23344,7 @@
     </row>
     <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B29" s="6">
         <v>4020</v>
@@ -23451,7 +23367,7 @@
     </row>
     <row r="30" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="B30" s="6">
         <v>4019</v>
@@ -23474,7 +23390,7 @@
     </row>
     <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="B31" s="6">
         <v>4031</v>
@@ -23497,7 +23413,7 @@
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="B32" s="6">
         <v>4032</v>
@@ -23520,7 +23436,7 @@
     </row>
     <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="B33" s="6">
         <v>4009</v>
@@ -23543,7 +23459,7 @@
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="B34" s="6">
         <v>4010</v>
@@ -23566,7 +23482,7 @@
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="B35" s="6">
         <v>4040</v>
@@ -23589,7 +23505,7 @@
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B36" s="6">
         <v>4039</v>
@@ -23612,7 +23528,7 @@
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="B37" s="6">
         <v>4024</v>
@@ -23635,7 +23551,7 @@
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="B38" s="6">
         <v>4023</v>
@@ -23658,7 +23574,7 @@
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="B39" s="6">
         <v>4016</v>
@@ -23681,7 +23597,7 @@
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B40" s="6">
         <v>4015</v>
@@ -23704,7 +23620,7 @@
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="B41" s="6">
         <v>4011</v>
@@ -23727,7 +23643,7 @@
     </row>
     <row r="42" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="B42" s="6">
         <v>4012</v>
@@ -23750,7 +23666,7 @@
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="B43" s="6">
         <v>4020</v>
@@ -23773,7 +23689,7 @@
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="B44" s="6">
         <v>4019</v>
@@ -23796,7 +23712,7 @@
     </row>
     <row r="45" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B45" s="6">
         <v>4031</v>
@@ -23819,7 +23735,7 @@
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="B46" s="6">
         <v>4032</v>
@@ -23842,7 +23758,7 @@
     </row>
     <row r="47" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B47" s="6">
         <v>4009</v>
@@ -23865,7 +23781,7 @@
     </row>
     <row r="48" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B48" s="6">
         <v>4010</v>
@@ -23888,7 +23804,7 @@
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B49" s="6">
         <v>4040</v>
@@ -23911,7 +23827,7 @@
     </row>
     <row r="50" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="B50" s="6">
         <v>4039</v>
@@ -23934,7 +23850,7 @@
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B51" s="6">
         <v>4024</v>
@@ -23957,7 +23873,7 @@
     </row>
     <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="B52" s="6">
         <v>4023</v>
@@ -23980,7 +23896,7 @@
     </row>
     <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="B53" s="6">
         <v>4016</v>
@@ -24003,7 +23919,7 @@
     </row>
     <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="B54" s="6">
         <v>4015</v>
@@ -24026,7 +23942,7 @@
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="B55" s="6">
         <v>4011</v>
@@ -24049,7 +23965,7 @@
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="B56" s="6">
         <v>4012</v>
@@ -24072,7 +23988,7 @@
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="B57" s="6">
         <v>4020</v>
@@ -24095,7 +24011,7 @@
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="B58" s="6">
         <v>4019</v>
@@ -24118,7 +24034,7 @@
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="B59" s="6">
         <v>4031</v>
@@ -24141,7 +24057,7 @@
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="B60" s="6">
         <v>4032</v>
@@ -24164,7 +24080,7 @@
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="B61" s="6">
         <v>4009</v>
@@ -24187,7 +24103,7 @@
     </row>
     <row r="62" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="B62" s="6">
         <v>4010</v>
@@ -24210,7 +24126,7 @@
     </row>
     <row r="63" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="B63" s="6">
         <v>4040</v>
@@ -24233,7 +24149,7 @@
     </row>
     <row r="64" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="B64" s="6">
         <v>4039</v>
@@ -24256,7 +24172,7 @@
     </row>
     <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="B65" s="6">
         <v>4024</v>
@@ -24279,7 +24195,7 @@
     </row>
     <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="B66" s="6">
         <v>4023</v>
@@ -24302,7 +24218,7 @@
     </row>
     <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="B67" s="6">
         <v>4016</v>
@@ -24325,7 +24241,7 @@
     </row>
     <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="B68" s="6">
         <v>4015</v>
@@ -24348,7 +24264,7 @@
     </row>
     <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="B69" s="6">
         <v>4011</v>
@@ -24371,7 +24287,7 @@
     </row>
     <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="B70" s="6">
         <v>4012</v>
@@ -24394,7 +24310,7 @@
     </row>
     <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B71" s="6">
         <v>4020</v>
@@ -24417,7 +24333,7 @@
     </row>
     <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B72" s="6">
         <v>4019</v>
@@ -24440,7 +24356,7 @@
     </row>
     <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="B73" s="6">
         <v>4031</v>
@@ -24463,7 +24379,7 @@
     </row>
     <row r="74" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="B74" s="6">
         <v>4032</v>
@@ -24486,7 +24402,7 @@
     </row>
     <row r="75" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="B75" s="6">
         <v>4009</v>
@@ -24509,7 +24425,7 @@
     </row>
     <row r="76" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B76" s="6">
         <v>4010</v>
@@ -24532,7 +24448,7 @@
     </row>
     <row r="77" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B77" s="6">
         <v>4040</v>
@@ -24555,7 +24471,7 @@
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="B78" s="6">
         <v>4039</v>
@@ -24578,7 +24494,7 @@
     </row>
     <row r="79" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="B79" s="6">
         <v>4024</v>
@@ -24601,7 +24517,7 @@
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="B80" s="6">
         <v>4023</v>
@@ -24624,7 +24540,7 @@
     </row>
     <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="B81" s="6">
         <v>4016</v>
@@ -24647,7 +24563,7 @@
     </row>
     <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="B82" s="6">
         <v>4015</v>
@@ -24670,7 +24586,7 @@
     </row>
     <row r="83" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="B83" s="6">
         <v>4011</v>
@@ -24693,7 +24609,7 @@
     </row>
     <row r="84" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="B84" s="6">
         <v>4012</v>
@@ -24716,7 +24632,7 @@
     </row>
     <row r="85" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="B85" s="6">
         <v>4020</v>
@@ -24739,7 +24655,7 @@
     </row>
     <row r="86" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="B86" s="6">
         <v>4019</v>
@@ -24762,7 +24678,7 @@
     </row>
     <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B87" s="6">
         <v>4031</v>
@@ -24785,7 +24701,7 @@
     </row>
     <row r="88" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="B88" s="6">
         <v>4032</v>
@@ -24808,7 +24724,7 @@
     </row>
     <row r="89" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="B89" s="6">
         <v>4009</v>
@@ -24831,7 +24747,7 @@
     </row>
     <row r="90" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="B90" s="6">
         <v>4010</v>
@@ -24854,7 +24770,7 @@
     </row>
     <row r="91" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B91" s="6">
         <v>4039</v>
@@ -24877,7 +24793,7 @@
     </row>
     <row r="92" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="B92" s="6">
         <v>4024</v>
@@ -24900,7 +24816,7 @@
     </row>
     <row r="93" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B93" s="6">
         <v>4023</v>
@@ -24923,7 +24839,7 @@
     </row>
     <row r="94" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B94" s="6">
         <v>4016</v>
@@ -24946,7 +24862,7 @@
     </row>
     <row r="95" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B95" s="6">
         <v>4015</v>
@@ -24969,7 +24885,7 @@
     </row>
     <row r="96" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B96" s="6">
         <v>4011</v>
@@ -24992,7 +24908,7 @@
     </row>
     <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B97" s="6">
         <v>4012</v>
@@ -25015,7 +24931,7 @@
     </row>
     <row r="98" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="B98" s="6">
         <v>4020</v>
@@ -25038,7 +24954,7 @@
     </row>
     <row r="99" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="B99" s="6">
         <v>4019</v>
@@ -25061,7 +24977,7 @@
     </row>
     <row r="100" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="B100" s="6">
         <v>4031</v>
@@ -25084,7 +25000,7 @@
     </row>
     <row r="101" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="B101" s="6">
         <v>4032</v>
@@ -25107,7 +25023,7 @@
     </row>
     <row r="102" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="B102" s="6">
         <v>4009</v>
@@ -25130,7 +25046,7 @@
     </row>
     <row r="103" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="B103" s="6">
         <v>4010</v>
@@ -25153,7 +25069,7 @@
     </row>
     <row r="104" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="B104" s="6">
         <v>4044</v>
@@ -25176,7 +25092,7 @@
     </row>
     <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="B105" s="6">
         <v>4043</v>
@@ -25199,7 +25115,7 @@
     </row>
     <row r="106" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B106" s="6">
         <v>4024</v>
@@ -25222,7 +25138,7 @@
     </row>
     <row r="107" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B107" s="6">
         <v>4023</v>
@@ -25245,7 +25161,7 @@
     </row>
     <row r="108" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B108" s="6">
         <v>4016</v>
@@ -25268,7 +25184,7 @@
     </row>
     <row r="109" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B109" s="6">
         <v>4015</v>
@@ -25291,7 +25207,7 @@
     </row>
     <row r="110" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="B110" s="6">
         <v>4011</v>
@@ -25314,7 +25230,7 @@
     </row>
     <row r="111" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="B111" s="6">
         <v>4012</v>
@@ -25337,7 +25253,7 @@
     </row>
     <row r="112" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B112" s="6">
         <v>4020</v>
@@ -25360,7 +25276,7 @@
     </row>
     <row r="113" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B113" s="6">
         <v>4019</v>
@@ -25383,7 +25299,7 @@
     </row>
     <row r="114" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B114" s="6">
         <v>4031</v>
@@ -25406,7 +25322,7 @@
     </row>
     <row r="115" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B115" s="6">
         <v>4032</v>
@@ -25429,7 +25345,7 @@
     </row>
     <row r="116" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="B116" s="6">
         <v>4009</v>
@@ -25452,7 +25368,7 @@
     </row>
     <row r="117" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B117" s="6">
         <v>4010</v>
@@ -25475,7 +25391,7 @@
     </row>
     <row r="118" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B118" s="6">
         <v>4044</v>
@@ -25498,7 +25414,7 @@
     </row>
     <row r="119" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B119" s="6">
         <v>4043</v>
@@ -25521,7 +25437,7 @@
     </row>
     <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B120" s="6">
         <v>4024</v>
@@ -25544,7 +25460,7 @@
     </row>
     <row r="121" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B121" s="6">
         <v>4023</v>
@@ -25567,7 +25483,7 @@
     </row>
     <row r="122" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B122" s="6">
         <v>4011</v>
@@ -25590,7 +25506,7 @@
     </row>
     <row r="123" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B123" s="6">
         <v>4012</v>
@@ -25614,7 +25530,7 @@
     </row>
     <row r="124" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B124" s="6">
         <v>4029</v>
@@ -25637,7 +25553,7 @@
     </row>
     <row r="125" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B125" s="6">
         <v>4030</v>
@@ -25662,7 +25578,7 @@
     </row>
     <row r="126" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B126" s="6">
         <v>4044</v>
@@ -25685,7 +25601,7 @@
     </row>
     <row r="127" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B127" s="6">
         <v>4043</v>
@@ -25708,7 +25624,7 @@
     </row>
     <row r="128" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B128" s="6">
         <v>4024</v>
@@ -25731,7 +25647,7 @@
     </row>
     <row r="129" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B129" s="6">
         <v>4023</v>
@@ -25751,12 +25667,12 @@
         <v>5.7997685187729076E-2</v>
       </c>
       <c r="G129" s="10" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="130" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B130" s="6">
         <v>4011</v>
@@ -25779,7 +25695,7 @@
     </row>
     <row r="131" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B131" s="6">
         <v>4012</v>
@@ -25802,7 +25718,7 @@
     </row>
     <row r="132" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B132" s="6">
         <v>4031</v>
@@ -25822,12 +25738,12 @@
         <v>5.0937500003783498E-2</v>
       </c>
       <c r="G132" s="10" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="133" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B133" s="6">
         <v>4044</v>
@@ -25846,12 +25762,12 @@
         <v>4.0034722216660157E-2</v>
       </c>
       <c r="G133" s="10" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="134" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B134" s="6">
         <v>4024</v>
@@ -25871,12 +25787,12 @@
         <v>2.5023148147738539E-2</v>
       </c>
       <c r="G134" s="10" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="135" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B135" s="6">
         <v>4011</v>
@@ -26206,18 +26122,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A120:B120">
-    <cfRule type="expression" dxfId="6" priority="240">
+    <cfRule type="expression" dxfId="14" priority="240">
       <formula>#REF!&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="241">
+    <cfRule type="expression" dxfId="13" priority="241">
       <formula>#REF!&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A133:B133">
-    <cfRule type="expression" dxfId="2" priority="256">
+    <cfRule type="expression" dxfId="12" priority="256">
       <formula>$P142&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="257">
+    <cfRule type="expression" dxfId="11" priority="257">
       <formula>$O142&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27837,7 +27753,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="54" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C10" s="61">
         <f>C76</f>
@@ -27846,7 +27762,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="54" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="C11" s="61">
         <f>C84</f>
@@ -27855,7 +27771,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="54" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="C12" s="61">
         <f>C92</f>
@@ -27864,7 +27780,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="54" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="C13" s="61">
         <f>C100</f>

</xml_diff>